<commit_message>
Added larger vector index
</commit_message>
<xml_diff>
--- a/aml/data/qa_dataset.xlsx
+++ b/aml/data/qa_dataset.xlsx
@@ -165,7 +165,7 @@
     <t>het kindje geboren is via een keizersnede</t>
   </si>
   <si>
-    <t>id</t>
+    <t>question_id</t>
   </si>
   <si>
     <t>group</t>
@@ -12416,14 +12416,14 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="2.5"/>
+    <col customWidth="1" min="1" max="1" width="9.13"/>
     <col customWidth="1" min="2" max="2" width="44.0"/>
     <col customWidth="1" min="3" max="3" width="76.13"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="17" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>52</v>

</xml_diff>